<commit_message>
Uppdatera trallgolv och lägg till trossbottenpapp med enhet m2 för golvyta-beräkning
</commit_message>
<xml_diff>
--- a/public/material_prislista.xlsx
+++ b/public/material_prislista.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -495,28 +495,28 @@
         <v>Golv</v>
       </c>
       <c r="B4" t="str">
-        <v>Trallgolv 120mm</v>
+        <v>Trallgolv</v>
       </c>
       <c r="C4" t="str">
-        <v>lm</v>
+        <v>m2</v>
       </c>
       <c r="D4">
-        <v>8.4</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>0.035</v>
+        <v>0.15</v>
       </c>
       <c r="F4">
-        <v>25</v>
+        <v>195</v>
       </c>
       <c r="G4">
-        <v>45</v>
+        <v>350</v>
       </c>
       <c r="H4" t="b">
         <v>1</v>
       </c>
       <c r="I4" t="str">
-        <v>9.52 lm/m²</v>
+        <v>Beräknas på golvyta</v>
       </c>
     </row>
     <row r="5">
@@ -553,7 +553,7 @@
         <v>Golv</v>
       </c>
       <c r="B6" t="str">
-        <v>Spånskivegolv</v>
+        <v>Trossbottenpapp</v>
       </c>
       <c r="C6" t="str">
         <v>m2</v>
@@ -562,19 +562,19 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F6">
-        <v>95</v>
+        <v>25</v>
       </c>
       <c r="G6">
-        <v>160</v>
+        <v>45</v>
       </c>
       <c r="H6" t="b">
         <v>1</v>
       </c>
       <c r="I6" t="str">
-        <v/>
+        <v>Beräknas på golvyta</v>
       </c>
     </row>
     <row r="7">
@@ -582,7 +582,7 @@
         <v>Golv</v>
       </c>
       <c r="B7" t="str">
-        <v>Isolering golv</v>
+        <v>Spånskivegolv</v>
       </c>
       <c r="C7" t="str">
         <v>m2</v>
@@ -591,27 +591,27 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="F7">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="G7">
-        <v>125</v>
+        <v>160</v>
       </c>
       <c r="H7" t="b">
         <v>1</v>
       </c>
       <c r="I7" t="str">
-        <v/>
+        <v>Beräknas på golvyta</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Stomme</v>
+        <v>Golv</v>
       </c>
       <c r="B8" t="str">
-        <v>Timmer (tillverkning)</v>
+        <v>Isolering golv</v>
       </c>
       <c r="C8" t="str">
         <v>m2</v>
@@ -620,19 +620,19 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <v>1.5</v>
+        <v>0.08</v>
       </c>
       <c r="F8">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="G8">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="H8" t="b">
         <v>1</v>
       </c>
       <c r="I8" t="str">
-        <v>Väggarea m² × pris/m</v>
+        <v>Beräknas på golvyta</v>
       </c>
     </row>
     <row r="9">
@@ -640,7 +640,7 @@
         <v>Stomme</v>
       </c>
       <c r="B9" t="str">
-        <v>Montering stomme</v>
+        <v>Timmer (tillverkning)</v>
       </c>
       <c r="C9" t="str">
         <v>m2</v>
@@ -649,19 +649,19 @@
         <v>1</v>
       </c>
       <c r="E9">
-        <v>0.8</v>
+        <v>1.5</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="H9" t="b">
         <v>1</v>
       </c>
       <c r="I9" t="str">
-        <v>Endast arbetstid</v>
+        <v>Väggarea m² × pris/m</v>
       </c>
     </row>
     <row r="10">
@@ -669,36 +669,36 @@
         <v>Stomme</v>
       </c>
       <c r="B10" t="str">
-        <v>Syllvirke 45x95</v>
+        <v>Montering stomme</v>
       </c>
       <c r="C10" t="str">
-        <v>lm</v>
+        <v>m2</v>
       </c>
       <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0.8</v>
+      </c>
+      <c r="F10">
         <v>0</v>
       </c>
-      <c r="E10">
-        <v>0.1</v>
-      </c>
-      <c r="F10">
-        <v>25</v>
-      </c>
       <c r="G10">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="H10" t="b">
         <v>1</v>
       </c>
       <c r="I10" t="str">
-        <v>Syllomkrets</v>
+        <v>Endast arbetstid</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Tak</v>
+        <v>Stomme</v>
       </c>
       <c r="B11" t="str">
-        <v>Takåsar</v>
+        <v>Syllvirke 45x95</v>
       </c>
       <c r="C11" t="str">
         <v>lm</v>
@@ -707,19 +707,19 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="F11">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="G11">
-        <v>150</v>
+        <v>45</v>
       </c>
       <c r="H11" t="b">
         <v>1</v>
       </c>
       <c r="I11" t="str">
-        <v>Antal × taklängd</v>
+        <v>Syllomkrets</v>
       </c>
     </row>
     <row r="12">
@@ -727,28 +727,28 @@
         <v>Tak</v>
       </c>
       <c r="B12" t="str">
-        <v>Råspont</v>
+        <v>Takåsar</v>
       </c>
       <c r="C12" t="str">
-        <v>m2</v>
+        <v>lm</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="F12">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="G12">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="H12" t="b">
         <v>1</v>
       </c>
       <c r="I12" t="str">
-        <v/>
+        <v>Antal × taklängd</v>
       </c>
     </row>
     <row r="13">
@@ -756,7 +756,7 @@
         <v>Tak</v>
       </c>
       <c r="B13" t="str">
-        <v>Underlagspapp</v>
+        <v>Råspont</v>
       </c>
       <c r="C13" t="str">
         <v>m2</v>
@@ -765,13 +765,13 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="F13">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="G13">
-        <v>55</v>
+        <v>165</v>
       </c>
       <c r="H13" t="b">
         <v>1</v>
@@ -785,28 +785,28 @@
         <v>Tak</v>
       </c>
       <c r="B14" t="str">
-        <v>Ströläkt 12x50</v>
+        <v>Underlagspapp</v>
       </c>
       <c r="C14" t="str">
-        <v>lm</v>
+        <v>m2</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="F14">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="G14">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="H14" t="b">
         <v>1</v>
       </c>
       <c r="I14" t="str">
-        <v>c/c 0.6</v>
+        <v/>
       </c>
     </row>
     <row r="15">
@@ -814,28 +814,28 @@
         <v>Tak</v>
       </c>
       <c r="B15" t="str">
-        <v>Bärläkt 28x70</v>
+        <v>Ströläkt 12x50</v>
       </c>
       <c r="C15" t="str">
         <v>lm</v>
       </c>
       <c r="D15">
-        <v>1.67</v>
+        <v>2</v>
       </c>
       <c r="E15">
-        <v>0.08</v>
+        <v>0.04</v>
       </c>
       <c r="F15">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G15">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H15" t="b">
         <v>1</v>
       </c>
       <c r="I15" t="str">
-        <v>c/c 0.35</v>
+        <v>c/c 0.6</v>
       </c>
     </row>
     <row r="16">
@@ -843,28 +843,28 @@
         <v>Tak</v>
       </c>
       <c r="B16" t="str">
-        <v>Takplåt</v>
+        <v>Bärläkt 28x70</v>
       </c>
       <c r="C16" t="str">
-        <v>m2</v>
+        <v>lm</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>1.67</v>
       </c>
       <c r="E16">
-        <v>0.25</v>
+        <v>0.08</v>
       </c>
       <c r="F16">
-        <v>120</v>
+        <v>12</v>
       </c>
       <c r="G16">
-        <v>195</v>
+        <v>22</v>
       </c>
       <c r="H16" t="b">
         <v>1</v>
       </c>
       <c r="I16" t="str">
-        <v/>
+        <v>c/c 0.35</v>
       </c>
     </row>
     <row r="17">
@@ -872,28 +872,28 @@
         <v>Tak</v>
       </c>
       <c r="B17" t="str">
-        <v>Fotplåt</v>
+        <v>Takplåt</v>
       </c>
       <c r="C17" t="str">
-        <v>lm</v>
+        <v>m2</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>0.12</v>
+        <v>0.25</v>
       </c>
       <c r="F17">
-        <v>45</v>
+        <v>120</v>
       </c>
       <c r="G17">
-        <v>75</v>
+        <v>195</v>
       </c>
       <c r="H17" t="b">
         <v>1</v>
       </c>
       <c r="I17" t="str">
-        <v>2 × taklängd</v>
+        <v/>
       </c>
     </row>
     <row r="18">
@@ -901,7 +901,7 @@
         <v>Tak</v>
       </c>
       <c r="B18" t="str">
-        <v>Vindskivor 22x145</v>
+        <v>Fotplåt</v>
       </c>
       <c r="C18" t="str">
         <v>lm</v>
@@ -910,19 +910,19 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="F18">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G18">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="H18" t="b">
         <v>1</v>
       </c>
       <c r="I18" t="str">
-        <v>4 × takfall</v>
+        <v>2 × taklängd</v>
       </c>
     </row>
     <row r="19">
@@ -930,7 +930,7 @@
         <v>Tak</v>
       </c>
       <c r="B19" t="str">
-        <v>Takfotsbräda 22x145</v>
+        <v>Vindskivor 22x145</v>
       </c>
       <c r="C19" t="str">
         <v>lm</v>
@@ -939,19 +939,19 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>0.15</v>
+        <v>0.4</v>
       </c>
       <c r="F19">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="G19">
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="H19" t="b">
         <v>1</v>
       </c>
       <c r="I19" t="str">
-        <v>2 × taklängd</v>
+        <v>4 × takfall</v>
       </c>
     </row>
     <row r="20">
@@ -959,7 +959,7 @@
         <v>Tak</v>
       </c>
       <c r="B20" t="str">
-        <v>Regnvattensystem</v>
+        <v>Takfotsbräda 22x145</v>
       </c>
       <c r="C20" t="str">
         <v>lm</v>
@@ -968,13 +968,13 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="F20">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="G20">
-        <v>145</v>
+        <v>45</v>
       </c>
       <c r="H20" t="b">
         <v>1</v>
@@ -988,7 +988,7 @@
         <v>Tak</v>
       </c>
       <c r="B21" t="str">
-        <v>Nockplåt</v>
+        <v>Regnvattensystem</v>
       </c>
       <c r="C21" t="str">
         <v>lm</v>
@@ -997,24 +997,53 @@
         <v>0</v>
       </c>
       <c r="E21">
+        <v>0.2</v>
+      </c>
+      <c r="F21">
+        <v>85</v>
+      </c>
+      <c r="G21">
+        <v>145</v>
+      </c>
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" t="str">
+        <v>2 × taklängd</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>Tak</v>
+      </c>
+      <c r="B22" t="str">
+        <v>Nockplåt</v>
+      </c>
+      <c r="C22" t="str">
+        <v>lm</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
         <v>0.1</v>
       </c>
-      <c r="F21">
+      <c r="F22">
         <v>65</v>
       </c>
-      <c r="G21">
+      <c r="G22">
         <v>110</v>
       </c>
-      <c r="H21" t="b">
-        <v>1</v>
-      </c>
-      <c r="I21" t="str">
+      <c r="H22" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" t="str">
         <v>Taklängd</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I21"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I22"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Vindskivor beräknas nu i antal (st) - MangdPerM2 anger antal brädor per takfallskant
</commit_message>
<xml_diff>
--- a/public/material_prislista.xlsx
+++ b/public/material_prislista.xlsx
@@ -933,10 +933,10 @@
         <v>Vindskivor 22x145</v>
       </c>
       <c r="C19" t="str">
-        <v>lm</v>
+        <v>st</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E19">
         <v>0.4</v>
@@ -951,7 +951,7 @@
         <v>1</v>
       </c>
       <c r="I19" t="str">
-        <v>4 × takfall</v>
+        <v>2 per kant × 4 kanter = 8 st (sadeltak)</v>
       </c>
     </row>
     <row r="20">

</xml_diff>

<commit_message>
Vindskivor: MangdPerM2 = antal brädor per sida, beräknas som (brädor × sidor × takfall) meter
</commit_message>
<xml_diff>
--- a/public/material_prislista.xlsx
+++ b/public/material_prislista.xlsx
@@ -933,10 +933,10 @@
         <v>Vindskivor 22x145</v>
       </c>
       <c r="C19" t="str">
-        <v>st</v>
+        <v>lm</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E19">
         <v>0.4</v>
@@ -951,7 +951,7 @@
         <v>1</v>
       </c>
       <c r="I19" t="str">
-        <v>2 per kant × 4 kanter = 8 st (sadeltak)</v>
+        <v>4 brädor/sida × takfall (sadeltak: 8×, pulpet: 4×)</v>
       </c>
     </row>
     <row r="20">

</xml_diff>

<commit_message>
Lägg till Vindskiveplåt - beräknas i antal (st) baserat på täckning per plåt
</commit_message>
<xml_diff>
--- a/public/material_prislista.xlsx
+++ b/public/material_prislista.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -959,28 +959,28 @@
         <v>Tak</v>
       </c>
       <c r="B20" t="str">
-        <v>Takfotsbräda 22x145</v>
+        <v>Vindskiveplåt</v>
       </c>
       <c r="C20" t="str">
-        <v>lm</v>
+        <v>st</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>1.9</v>
       </c>
       <c r="E20">
         <v>0.15</v>
       </c>
       <c r="F20">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="G20">
-        <v>45</v>
+        <v>145</v>
       </c>
       <c r="H20" t="b">
         <v>1</v>
       </c>
       <c r="I20" t="str">
-        <v>2 × taklängd</v>
+        <v>Täcker 1.9m/st, avrundas uppåt</v>
       </c>
     </row>
     <row r="21">
@@ -988,7 +988,7 @@
         <v>Tak</v>
       </c>
       <c r="B21" t="str">
-        <v>Regnvattensystem</v>
+        <v>Takfotsbräda 22x145</v>
       </c>
       <c r="C21" t="str">
         <v>lm</v>
@@ -997,13 +997,13 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="F21">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="G21">
-        <v>145</v>
+        <v>45</v>
       </c>
       <c r="H21" t="b">
         <v>1</v>
@@ -1017,7 +1017,7 @@
         <v>Tak</v>
       </c>
       <c r="B22" t="str">
-        <v>Nockplåt</v>
+        <v>Regnvattensystem</v>
       </c>
       <c r="C22" t="str">
         <v>lm</v>
@@ -1026,24 +1026,53 @@
         <v>0</v>
       </c>
       <c r="E22">
+        <v>0.2</v>
+      </c>
+      <c r="F22">
+        <v>85</v>
+      </c>
+      <c r="G22">
+        <v>145</v>
+      </c>
+      <c r="H22" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" t="str">
+        <v>2 × taklängd</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>Tak</v>
+      </c>
+      <c r="B23" t="str">
+        <v>Nockplåt</v>
+      </c>
+      <c r="C23" t="str">
+        <v>lm</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
         <v>0.1</v>
       </c>
-      <c r="F22">
+      <c r="F23">
         <v>65</v>
       </c>
-      <c r="G22">
+      <c r="G23">
         <v>110</v>
       </c>
-      <c r="H22" t="b">
-        <v>1</v>
-      </c>
-      <c r="I22" t="str">
+      <c r="H23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" t="str">
         <v>Taklängd</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I22"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I23"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Rätta vindskivor/vindskiveplåt: använd antal takfall (4 sadeltak, 2 pulpettak)
</commit_message>
<xml_diff>
--- a/public/material_prislista.xlsx
+++ b/public/material_prislista.xlsx
@@ -936,7 +936,7 @@
         <v>lm</v>
       </c>
       <c r="D19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E19">
         <v>0.4</v>
@@ -951,7 +951,7 @@
         <v>1</v>
       </c>
       <c r="I19" t="str">
-        <v>4 brädor/sida × takfall (sadeltak: 8×, pulpet: 4×)</v>
+        <v>2 brädor/takfall (sadeltak: 4×2=8, pulpet: 2×2=4)</v>
       </c>
     </row>
     <row r="20">
@@ -980,7 +980,7 @@
         <v>1</v>
       </c>
       <c r="I20" t="str">
-        <v>Täcker 1.9m/st, avrundas uppåt</v>
+        <v>Täcker 1.9m/st (sadeltak: 4 takfall, pulpet: 2)</v>
       </c>
     </row>
     <row r="21">

</xml_diff>

<commit_message>
Fotplåt: ändra till st med täckning 1.9m (sadeltak 2 sidor, pulpet 1 sida)
</commit_message>
<xml_diff>
--- a/public/material_prislista.xlsx
+++ b/public/material_prislista.xlsx
@@ -904,10 +904,10 @@
         <v>Fotplåt</v>
       </c>
       <c r="C18" t="str">
-        <v>lm</v>
+        <v>st</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>1.9</v>
       </c>
       <c r="E18">
         <v>0.12</v>
@@ -922,7 +922,7 @@
         <v>1</v>
       </c>
       <c r="I18" t="str">
-        <v>2 × taklängd</v>
+        <v>Täcker 1.9m/st (sadeltak: 2 sidor, pulpet: 1 sida)</v>
       </c>
     </row>
     <row r="19">

</xml_diff>

<commit_message>
Ändra timmerenhet från kr/m till kr/m² i Sidebar och Ekonomi-script
</commit_message>
<xml_diff>
--- a/public/material_prislista.xlsx
+++ b/public/material_prislista.xlsx
@@ -1,42 +1,222 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rogerwagenius/Documents/Programmering/Timmer26/public/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13248001-09E4-A548-859E-09AB3488E845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Material" sheetId="1" r:id="rId1"/>
     <sheet name="Ekonomi" sheetId="2" r:id="rId2"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="63">
+  <si>
+    <t>Kategori</t>
+  </si>
+  <si>
+    <t>Artikel</t>
+  </si>
+  <si>
+    <t>Enhet</t>
+  </si>
+  <si>
+    <t>MangdPerM2</t>
+  </si>
+  <si>
+    <t>Enhetstid</t>
+  </si>
+  <si>
+    <t>Inkopspris</t>
+  </si>
+  <si>
+    <t>Forsaljningspris</t>
+  </si>
+  <si>
+    <t>TaMed</t>
+  </si>
+  <si>
+    <t>Notering</t>
+  </si>
+  <si>
+    <t>Golv</t>
+  </si>
+  <si>
+    <t>Golvreglar 45x145-220</t>
+  </si>
+  <si>
+    <t>lm</t>
+  </si>
+  <si>
+    <t>Impregnerad</t>
+  </si>
+  <si>
+    <t>Stödregel 45x45</t>
+  </si>
+  <si>
+    <t>Trallgolv</t>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <t>Beräknas på golvyta</t>
+  </si>
+  <si>
+    <t>Trossbottenskiva</t>
+  </si>
+  <si>
+    <t>st</t>
+  </si>
+  <si>
+    <t>0.72 m²/skiva, avrundas uppåt</t>
+  </si>
+  <si>
+    <t>Trossbottenpapp</t>
+  </si>
+  <si>
+    <t>Spånskivegolv</t>
+  </si>
+  <si>
+    <t>Isolering golv</t>
+  </si>
+  <si>
+    <t>Stomme</t>
+  </si>
+  <si>
+    <t>Timmer (tillverkning)</t>
+  </si>
+  <si>
+    <t>Väggarea m² × pris/m</t>
+  </si>
+  <si>
+    <t>Montering stomme</t>
+  </si>
+  <si>
+    <t>Endast arbetstid</t>
+  </si>
+  <si>
+    <t>Syllvirke 45x95</t>
+  </si>
+  <si>
+    <t>Syllomkrets</t>
+  </si>
+  <si>
+    <t>Tak</t>
+  </si>
+  <si>
+    <t>Takåsar</t>
+  </si>
+  <si>
+    <t>Antal × taklängd</t>
+  </si>
+  <si>
+    <t>Råspont</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Underlagspapp</t>
+  </si>
+  <si>
+    <t>Ströläkt 12x50</t>
+  </si>
+  <si>
+    <t>c/c 0.6</t>
+  </si>
+  <si>
+    <t>Bärläkt 28x70</t>
+  </si>
+  <si>
+    <t>Takplåt</t>
+  </si>
+  <si>
+    <t>Fotplåt</t>
+  </si>
+  <si>
+    <t>Täcker 1.9m/st (sadeltak: 2 sidor, pulpet: 1 sida)</t>
+  </si>
+  <si>
+    <t>Vindskivor 22x145</t>
+  </si>
+  <si>
+    <t>2 brädor/takfall (sadeltak: 4×2=8, pulpet: 2×2=4)</t>
+  </si>
+  <si>
+    <t>Vindskiveplåt</t>
+  </si>
+  <si>
+    <t>Täcker 1.9m/st (sadeltak: 4 takfall, pulpet: 2)</t>
+  </si>
+  <si>
+    <t>Takfotsbräda 22x145</t>
+  </si>
+  <si>
+    <t>2 × taklängd</t>
+  </si>
+  <si>
+    <t>Regnvattensystem</t>
+  </si>
+  <si>
+    <t>Nockplåt</t>
+  </si>
+  <si>
+    <t>Taklängd</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Värde</t>
+  </si>
+  <si>
+    <t>Beskrivning</t>
+  </si>
+  <si>
+    <t>PrisTimmerIn</t>
+  </si>
+  <si>
+    <t>Inköpspris timmer (kr/m)</t>
+  </si>
+  <si>
+    <t>PrisTimmerUt</t>
+  </si>
+  <si>
+    <t>Försäljningspris timmer (kr/m)</t>
+  </si>
+  <si>
+    <t>Timkostnad</t>
+  </si>
+  <si>
+    <t>Timkostnad (kr/h)</t>
+  </si>
+  <si>
+    <t>MomsPct</t>
+  </si>
+  <si>
+    <t>Moms (%)</t>
+  </si>
+  <si>
+    <t>c/c 0.5</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -66,13 +246,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -397,50 +585,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Kategori</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Artikel</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Enhet</v>
-      </c>
-      <c r="D1" t="str">
-        <v>MangdPerM2</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Enhetstid</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Inkopspris</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Forsaljningspris</v>
-      </c>
-      <c r="H1" t="str">
-        <v>TaMed</v>
-      </c>
-      <c r="I1" t="str">
-        <v>Notering</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Golv</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Golvreglar 45x145-220</v>
-      </c>
-      <c r="C2" t="str">
-        <v>lm</v>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
       </c>
       <c r="D2">
         <v>1.67</v>
@@ -457,19 +651,19 @@
       <c r="H2" t="b">
         <v>1</v>
       </c>
-      <c r="I2" t="str">
-        <v>Impregnerad</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Golv</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Stödregel 45x45</v>
-      </c>
-      <c r="C3" t="str">
-        <v>lm</v>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
       </c>
       <c r="D3">
         <v>0.41</v>
@@ -486,19 +680,19 @@
       <c r="H3" t="b">
         <v>1</v>
       </c>
-      <c r="I3" t="str">
-        <v>Impregnerad</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Golv</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Trallgolv</v>
-      </c>
-      <c r="C4" t="str">
-        <v>m2</v>
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -515,25 +709,25 @@
       <c r="H4" t="b">
         <v>1</v>
       </c>
-      <c r="I4" t="str">
-        <v>Beräknas på golvyta</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Golv</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Trossbottenskiva</v>
-      </c>
-      <c r="C5" t="str">
-        <v>st</v>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
       </c>
       <c r="D5">
         <v>1.389</v>
       </c>
       <c r="E5">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="F5">
         <v>85</v>
@@ -544,19 +738,19 @@
       <c r="H5" t="b">
         <v>1</v>
       </c>
-      <c r="I5" t="str">
-        <v>0.72 m²/skiva, avrundas uppåt</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Golv</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Trossbottenpapp</v>
-      </c>
-      <c r="C6" t="str">
-        <v>m2</v>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -573,25 +767,25 @@
       <c r="H6" t="b">
         <v>1</v>
       </c>
-      <c r="I6" t="str">
-        <v>Beräknas på golvyta</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Golv</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Spånskivegolv</v>
-      </c>
-      <c r="C7" t="str">
-        <v>m2</v>
+      <c r="I6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="F7">
         <v>95</v>
@@ -602,25 +796,25 @@
       <c r="H7" t="b">
         <v>1</v>
       </c>
-      <c r="I7" t="str">
-        <v>Beräknas på golvyta</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>Golv</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Isolering golv</v>
-      </c>
-      <c r="C8" t="str">
-        <v>m2</v>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8">
-        <v>0.08</v>
+        <v>0.18</v>
       </c>
       <c r="F8">
         <v>75</v>
@@ -631,54 +825,54 @@
       <c r="H8" t="b">
         <v>1</v>
       </c>
-      <c r="I8" t="str">
-        <v>Beräknas på golvyta</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>Stomme</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Timmer (tillverkning)</v>
-      </c>
-      <c r="C9" t="str">
-        <v>m2</v>
+      <c r="I8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9">
-        <v>1.5</v>
+        <v>0.45</v>
       </c>
       <c r="F9">
-        <v>60</v>
+        <v>458</v>
       </c>
       <c r="G9">
-        <v>120</v>
+        <v>850</v>
       </c>
       <c r="H9" t="b">
         <v>1</v>
       </c>
-      <c r="I9" t="str">
-        <v>Väggarea m² × pris/m</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>Stomme</v>
-      </c>
-      <c r="B10" t="str">
-        <v>Montering stomme</v>
-      </c>
-      <c r="C10" t="str">
-        <v>m2</v>
+      <c r="I9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -689,19 +883,19 @@
       <c r="H10" t="b">
         <v>1</v>
       </c>
-      <c r="I10" t="str">
-        <v>Endast arbetstid</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>Stomme</v>
-      </c>
-      <c r="B11" t="str">
-        <v>Syllvirke 45x95</v>
-      </c>
-      <c r="C11" t="str">
-        <v>lm</v>
+      <c r="I10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -718,19 +912,19 @@
       <c r="H11" t="b">
         <v>1</v>
       </c>
-      <c r="I11" t="str">
-        <v>Syllomkrets</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>Tak</v>
-      </c>
-      <c r="B12" t="str">
-        <v>Takåsar</v>
-      </c>
-      <c r="C12" t="str">
-        <v>lm</v>
+      <c r="I11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -747,19 +941,19 @@
       <c r="H12" t="b">
         <v>1</v>
       </c>
-      <c r="I12" t="str">
-        <v>Antal × taklängd</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>Tak</v>
-      </c>
-      <c r="B13" t="str">
-        <v>Råspont</v>
-      </c>
-      <c r="C13" t="str">
-        <v>m2</v>
+      <c r="I12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -776,25 +970,25 @@
       <c r="H13" t="b">
         <v>1</v>
       </c>
-      <c r="I13" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>Tak</v>
-      </c>
-      <c r="B14" t="str">
-        <v>Underlagspapp</v>
-      </c>
-      <c r="C14" t="str">
-        <v>m2</v>
+      <c r="I13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="F14">
         <v>35</v>
@@ -805,25 +999,25 @@
       <c r="H14" t="b">
         <v>1</v>
       </c>
-      <c r="I14" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>Tak</v>
-      </c>
-      <c r="B15" t="str">
-        <v>Ströläkt 12x50</v>
-      </c>
-      <c r="C15" t="str">
-        <v>lm</v>
+      <c r="I14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
       </c>
       <c r="D15">
         <v>2</v>
       </c>
       <c r="E15">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="F15">
         <v>8</v>
@@ -834,25 +1028,25 @@
       <c r="H15" t="b">
         <v>1</v>
       </c>
-      <c r="I15" t="str">
-        <v>c/c 0.6</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="str">
-        <v>Tak</v>
-      </c>
-      <c r="B16" t="str">
-        <v>Bärläkt 28x70</v>
-      </c>
-      <c r="C16" t="str">
-        <v>lm</v>
+      <c r="I15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
       </c>
       <c r="D16">
         <v>1.67</v>
       </c>
       <c r="E16">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="F16">
         <v>12</v>
@@ -863,25 +1057,25 @@
       <c r="H16" t="b">
         <v>1</v>
       </c>
-      <c r="I16" t="str">
-        <v>c/c 0.35</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="str">
-        <v>Tak</v>
-      </c>
-      <c r="B17" t="str">
-        <v>Takplåt</v>
-      </c>
-      <c r="C17" t="str">
-        <v>m2</v>
+      <c r="I16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="F17">
         <v>120</v>
@@ -892,19 +1086,19 @@
       <c r="H17" t="b">
         <v>1</v>
       </c>
-      <c r="I17" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="str">
-        <v>Tak</v>
-      </c>
-      <c r="B18" t="str">
-        <v>Fotplåt</v>
-      </c>
-      <c r="C18" t="str">
-        <v>st</v>
+      <c r="I17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
       </c>
       <c r="D18">
         <v>1.9</v>
@@ -921,25 +1115,25 @@
       <c r="H18" t="b">
         <v>1</v>
       </c>
-      <c r="I18" t="str">
-        <v>Täcker 1.9m/st (sadeltak: 2 sidor, pulpet: 1 sida)</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="str">
-        <v>Tak</v>
-      </c>
-      <c r="B19" t="str">
-        <v>Vindskivor 22x145</v>
-      </c>
-      <c r="C19" t="str">
-        <v>lm</v>
+      <c r="I18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
       </c>
       <c r="D19">
         <v>2</v>
       </c>
       <c r="E19">
-        <v>0.4</v>
+        <v>0.15</v>
       </c>
       <c r="F19">
         <v>55</v>
@@ -950,25 +1144,25 @@
       <c r="H19" t="b">
         <v>1</v>
       </c>
-      <c r="I19" t="str">
-        <v>2 brädor/takfall (sadeltak: 4×2=8, pulpet: 2×2=4)</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="str">
-        <v>Tak</v>
-      </c>
-      <c r="B20" t="str">
-        <v>Vindskiveplåt</v>
-      </c>
-      <c r="C20" t="str">
-        <v>st</v>
+      <c r="I19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
       </c>
       <c r="D20">
         <v>1.9</v>
       </c>
       <c r="E20">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="F20">
         <v>85</v>
@@ -979,19 +1173,19 @@
       <c r="H20" t="b">
         <v>1</v>
       </c>
-      <c r="I20" t="str">
-        <v>Täcker 1.9m/st (sadeltak: 4 takfall, pulpet: 2)</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="str">
-        <v>Tak</v>
-      </c>
-      <c r="B21" t="str">
-        <v>Takfotsbräda 22x145</v>
-      </c>
-      <c r="C21" t="str">
-        <v>lm</v>
+      <c r="I20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1008,19 +1202,19 @@
       <c r="H21" t="b">
         <v>1</v>
       </c>
-      <c r="I21" t="str">
-        <v>2 × taklängd</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="str">
-        <v>Tak</v>
-      </c>
-      <c r="B22" t="str">
-        <v>Regnvattensystem</v>
-      </c>
-      <c r="C22" t="str">
-        <v>lm</v>
+      <c r="I21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1037,25 +1231,25 @@
       <c r="H22" t="b">
         <v>1</v>
       </c>
-      <c r="I22" t="str">
-        <v>2 × taklängd</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="str">
-        <v>Tak</v>
-      </c>
-      <c r="B23" t="str">
-        <v>Nockplåt</v>
-      </c>
-      <c r="C23" t="str">
-        <v>lm</v>
+      <c r="I22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="F23">
         <v>65</v>
@@ -1066,82 +1260,85 @@
       <c r="H23" t="b">
         <v>1</v>
       </c>
-      <c r="I23" t="str">
-        <v>Taklängd</v>
+      <c r="I23" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I23"/>
+    <ignoredError sqref="A1:I4 A18:I18 A14:D14 F14:I14 A15:D15 F15:I15 A16:D16 F16:H16 A17:D17 F17:I17 A21:I22 A20:D20 F20:I20 A19:D19 F19:I19 A23:D23 F23:I23 A11:I13 A9:D9 H9:I9 A10:D10 F10:I10 A6:I6 A5:D5 F5:I5 A8:D8 A7:D7 F7:I7 F8:I8" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Parameter</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Värde</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Beskrivning</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>PrisTimmerIn</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>54</v>
       </c>
       <c r="B2">
         <v>60</v>
       </c>
-      <c r="C2" t="str">
-        <v>Inköpspris timmer (kr/m)</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>PrisTimmerUt</v>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>56</v>
       </c>
       <c r="B3">
         <v>120</v>
       </c>
-      <c r="C3" t="str">
-        <v>Försäljningspris timmer (kr/m)</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Timkostnad</v>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>58</v>
       </c>
       <c r="B4">
         <v>450</v>
       </c>
-      <c r="C4" t="str">
-        <v>Timkostnad (kr/h)</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>MomsPct</v>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>60</v>
       </c>
       <c r="B5">
         <v>25</v>
       </c>
-      <c r="C5" t="str">
-        <v>Moms (%)</v>
+      <c r="C5" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
+    <ignoredError sqref="A1:C5" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Synka createExcel.mjs med alla värden från nuvarande Excel-fil
</commit_message>
<xml_diff>
--- a/public/material_prislista.xlsx
+++ b/public/material_prislista.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rogerwagenius/Documents/Programmering/Timmer26/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13248001-09E4-A548-859E-09AB3488E845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A108EED-5F15-3847-8999-FBEFA33C40C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="21360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Material" sheetId="1" r:id="rId1"/>
@@ -188,15 +188,9 @@
     <t>PrisTimmerIn</t>
   </si>
   <si>
-    <t>Inköpspris timmer (kr/m)</t>
-  </si>
-  <si>
     <t>PrisTimmerUt</t>
   </si>
   <si>
-    <t>Försäljningspris timmer (kr/m)</t>
-  </si>
-  <si>
     <t>Timkostnad</t>
   </si>
   <si>
@@ -210,6 +204,12 @@
   </si>
   <si>
     <t>c/c 0.5</t>
+  </si>
+  <si>
+    <t>Inköpspris timmer (kr/m2)</t>
+  </si>
+  <si>
+    <t>Försäljningspris timmer (kr/m2)</t>
   </si>
 </sst>
 </file>
@@ -588,7 +588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -1058,7 +1058,7 @@
         <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -1276,9 +1276,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1296,49 +1301,49 @@
         <v>54</v>
       </c>
       <c r="B2">
-        <v>60</v>
+        <v>458</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3">
-        <v>120</v>
+        <v>850</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B4">
-        <v>450</v>
+        <v>550</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B5">
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:C5" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:C1 A5:C5 A2 A3 A4 C4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Stor uppdatering: Grund, PDF/Word-export, ikoner och förbättringar
- Lagt till Grund-kategori med Plintar (9 st) och Betongsten (15 st)
- Lagt till Bärlina 45x95 för grundkonstruktion
- PDF-export (rapport) med logga, projekt och materialspecifikation
- Word-export (offert) med kundinfo och kategoribeskrivningar
- Spill% och Påslag% ersätter försäljningspris i Material-tabben
- Uppdaterade ikoner (🏗️ byggarbete, ⚙️ inställningar, 📐 material, 🧱 grund)
- Kompaktare layout i Stomme & bygghöjd
- Tid visas nu i timmar och minuter (t.ex. "2h 30min")
- Ytterarea visas i beräkningar
- Projektnamn-fält tillagt
- Kollapsbar sidebar
</commit_message>
<xml_diff>
--- a/public/material_prislista.xlsx
+++ b/public/material_prislista.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rogerwagenius/Documents/Programmering/Timmer26/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A108EED-5F15-3847-8999-FBEFA33C40C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5E9679-A198-824F-9207-44666CE6393C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="21360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="28800" windowHeight="17960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Material" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="73">
   <si>
     <t>Kategori</t>
   </si>
@@ -41,7 +41,10 @@
     <t>Inkopspris</t>
   </si>
   <si>
-    <t>Forsaljningspris</t>
+    <t>SpillPct</t>
+  </si>
+  <si>
+    <t>PaslagPct</t>
   </si>
   <si>
     <t>TaMed</t>
@@ -92,13 +95,19 @@
     <t>Isolering golv</t>
   </si>
   <si>
+    <t>Bärlina 45x95</t>
+  </si>
+  <si>
+    <t>Stommens bredd, för betongstensgrund</t>
+  </si>
+  <si>
     <t>Stomme</t>
   </si>
   <si>
     <t>Timmer (tillverkning)</t>
   </si>
   <si>
-    <t>Väggarea m² × pris/m</t>
+    <t>Pris inkl. tillverkning (~27min/m²)</t>
   </si>
   <si>
     <t>Montering stomme</t>
@@ -113,6 +122,12 @@
     <t>Syllomkrets</t>
   </si>
   <si>
+    <t>Dragstång</t>
+  </si>
+  <si>
+    <t>Fast antal: 6 st</t>
+  </si>
+  <si>
     <t>Tak</t>
   </si>
   <si>
@@ -140,6 +155,9 @@
     <t>Bärläkt 28x70</t>
   </si>
   <si>
+    <t>c/c 0.5</t>
+  </si>
+  <si>
     <t>Takplåt</t>
   </si>
   <si>
@@ -176,6 +194,21 @@
     <t>Taklängd</t>
   </si>
   <si>
+    <t>Grund</t>
+  </si>
+  <si>
+    <t>Plintar</t>
+  </si>
+  <si>
+    <t>20cm höga, c/c baserat på golvreglar</t>
+  </si>
+  <si>
+    <t>Betongsten 40x40x10</t>
+  </si>
+  <si>
+    <t>2 st staplade = 20cm höjd</t>
+  </si>
+  <si>
     <t>Parameter</t>
   </si>
   <si>
@@ -188,9 +221,15 @@
     <t>PrisTimmerIn</t>
   </si>
   <si>
+    <t>Inköpspris timmer (kr/m²)</t>
+  </si>
+  <si>
     <t>PrisTimmerUt</t>
   </si>
   <si>
+    <t>Försäljningspris timmer (kr/m²)</t>
+  </si>
+  <si>
     <t>Timkostnad</t>
   </si>
   <si>
@@ -201,15 +240,6 @@
   </si>
   <si>
     <t>Moms (%)</t>
-  </si>
-  <si>
-    <t>c/c 0.5</t>
-  </si>
-  <si>
-    <t>Inköpspris timmer (kr/m2)</t>
-  </si>
-  <si>
-    <t>Försäljningspris timmer (kr/m2)</t>
   </si>
 </sst>
 </file>
@@ -586,18 +616,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -625,16 +652,19 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2">
         <v>1.67</v>
@@ -646,53 +676,59 @@
         <v>45</v>
       </c>
       <c r="G2">
-        <v>85</v>
-      </c>
-      <c r="H2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>30</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
       <c r="D3">
-        <v>0.41</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>0.06</v>
       </c>
       <c r="F3">
+        <v>12</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>30</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="G3">
-        <v>30</v>
-      </c>
-      <c r="H3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -704,24 +740,27 @@
         <v>195</v>
       </c>
       <c r="G4">
-        <v>350</v>
-      </c>
-      <c r="H4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>30</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D5">
         <v>1.389</v>
@@ -733,24 +772,27 @@
         <v>85</v>
       </c>
       <c r="G5">
-        <v>145</v>
-      </c>
-      <c r="H5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>30</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -762,24 +804,27 @@
         <v>25</v>
       </c>
       <c r="G6">
-        <v>45</v>
-      </c>
-      <c r="H6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>30</v>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -791,24 +836,27 @@
         <v>95</v>
       </c>
       <c r="G7">
-        <v>160</v>
-      </c>
-      <c r="H7" t="b">
-        <v>1</v>
-      </c>
-      <c r="I7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>30</v>
+      </c>
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -820,454 +868,630 @@
         <v>75</v>
       </c>
       <c r="G8">
-        <v>125</v>
-      </c>
-      <c r="H8" t="b">
-        <v>1</v>
-      </c>
-      <c r="I8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="H8">
+        <v>30</v>
+      </c>
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
         <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>0.45</v>
+        <v>0.1</v>
       </c>
       <c r="F9">
+        <v>25</v>
+      </c>
+      <c r="G9">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <v>30</v>
+      </c>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
         <v>458</v>
       </c>
-      <c r="G9">
-        <v>850</v>
-      </c>
-      <c r="H9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>86</v>
+      </c>
+      <c r="I10" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>26</v>
       </c>
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
         <v>0.4</v>
       </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10" t="b">
-        <v>1</v>
-      </c>
-      <c r="I10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0.1</v>
-      </c>
       <c r="F11">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>45</v>
-      </c>
-      <c r="H11" t="b">
-        <v>1</v>
-      </c>
-      <c r="I11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
         <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="F12">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="G12">
-        <v>150</v>
-      </c>
-      <c r="H12" t="b">
-        <v>1</v>
-      </c>
-      <c r="I12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <v>30</v>
+      </c>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
         <v>33</v>
       </c>
       <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0.15</v>
+      </c>
+      <c r="F13">
+        <v>90</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
         <v>15</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
+      <c r="I13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0.15</v>
+      </c>
+      <c r="F14">
+        <v>85</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>30</v>
+      </c>
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
         <v>0.2</v>
       </c>
-      <c r="F13">
+      <c r="F15">
         <v>95</v>
       </c>
-      <c r="G13">
-        <v>165</v>
-      </c>
-      <c r="H13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="G15">
+        <v>10</v>
+      </c>
+      <c r="H15">
+        <v>30</v>
+      </c>
+      <c r="I15" t="b">
+        <v>1</v>
+      </c>
+      <c r="J15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>35</v>
       </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
         <v>0.08</v>
       </c>
-      <c r="F14">
+      <c r="F16">
         <v>35</v>
       </c>
-      <c r="G14">
-        <v>55</v>
-      </c>
-      <c r="H14" t="b">
-        <v>1</v>
-      </c>
-      <c r="I14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15">
+      <c r="G16">
+        <v>5</v>
+      </c>
+      <c r="H16">
+        <v>30</v>
+      </c>
+      <c r="I16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17">
         <v>2</v>
       </c>
-      <c r="E15">
+      <c r="E17">
         <v>0.05</v>
       </c>
-      <c r="F15">
+      <c r="F17">
         <v>8</v>
       </c>
-      <c r="G15">
-        <v>15</v>
-      </c>
-      <c r="H15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16">
+      <c r="G17">
+        <v>10</v>
+      </c>
+      <c r="H17">
+        <v>30</v>
+      </c>
+      <c r="I17" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18">
         <v>1.67</v>
       </c>
-      <c r="E16">
+      <c r="E18">
         <v>0.1</v>
       </c>
-      <c r="F16">
+      <c r="F18">
         <v>12</v>
       </c>
-      <c r="G16">
-        <v>22</v>
-      </c>
-      <c r="H16" t="b">
-        <v>1</v>
-      </c>
-      <c r="I16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="G18">
+        <v>10</v>
+      </c>
+      <c r="H18">
+        <v>30</v>
+      </c>
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
+      <c r="J18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>0.3</v>
+      </c>
+      <c r="F19">
+        <v>120</v>
+      </c>
+      <c r="G19">
+        <v>5</v>
+      </c>
+      <c r="H19">
+        <v>30</v>
+      </c>
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J19" t="s">
         <v>39</v>
       </c>
-      <c r="C17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>0.3</v>
-      </c>
-      <c r="F17">
-        <v>120</v>
-      </c>
-      <c r="G17">
-        <v>195</v>
-      </c>
-      <c r="H17" t="b">
-        <v>1</v>
-      </c>
-      <c r="I17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18">
-        <v>1.9</v>
-      </c>
-      <c r="E18">
-        <v>0.12</v>
-      </c>
-      <c r="F18">
-        <v>45</v>
-      </c>
-      <c r="G18">
-        <v>75</v>
-      </c>
-      <c r="H18" t="b">
-        <v>1</v>
-      </c>
-      <c r="I18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19">
-        <v>2</v>
-      </c>
-      <c r="E19">
-        <v>0.15</v>
-      </c>
-      <c r="F19">
-        <v>55</v>
-      </c>
-      <c r="G19">
-        <v>95</v>
-      </c>
-      <c r="H19" t="b">
-        <v>1</v>
-      </c>
-      <c r="I19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D20">
         <v>1.9</v>
       </c>
       <c r="E20">
-        <v>0.25</v>
+        <v>0.12</v>
       </c>
       <c r="F20">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="G20">
-        <v>145</v>
-      </c>
-      <c r="H20" t="b">
-        <v>1</v>
-      </c>
-      <c r="I20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="H20">
+        <v>30</v>
+      </c>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E21">
         <v>0.15</v>
       </c>
       <c r="F21">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="G21">
-        <v>45</v>
-      </c>
-      <c r="H21" t="b">
-        <v>1</v>
-      </c>
-      <c r="I21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="H21">
+        <v>30</v>
+      </c>
+      <c r="I21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C22" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>1.9</v>
       </c>
       <c r="E22">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="F22">
         <v>85</v>
       </c>
       <c r="G22">
-        <v>145</v>
-      </c>
-      <c r="H22" t="b">
-        <v>1</v>
-      </c>
-      <c r="I22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="H22">
+        <v>30</v>
+      </c>
+      <c r="I22" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23">
+        <v>0.15</v>
+      </c>
+      <c r="F23">
+        <v>25</v>
+      </c>
+      <c r="G23">
+        <v>10</v>
+      </c>
+      <c r="H23">
+        <v>30</v>
+      </c>
+      <c r="I23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0.2</v>
+      </c>
+      <c r="F24">
+        <v>85</v>
+      </c>
+      <c r="G24">
+        <v>5</v>
+      </c>
+      <c r="H24">
+        <v>30</v>
+      </c>
+      <c r="I24" t="b">
+        <v>0</v>
+      </c>
+      <c r="J24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
         <v>0.25</v>
       </c>
-      <c r="F23">
+      <c r="F25">
         <v>65</v>
       </c>
-      <c r="G23">
-        <v>110</v>
-      </c>
-      <c r="H23" t="b">
-        <v>1</v>
-      </c>
-      <c r="I23" t="s">
-        <v>50</v>
+      <c r="G25">
+        <v>5</v>
+      </c>
+      <c r="H25">
+        <v>30</v>
+      </c>
+      <c r="I25" t="b">
+        <v>1</v>
+      </c>
+      <c r="J25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0.15</v>
+      </c>
+      <c r="F26">
+        <v>150</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>30</v>
+      </c>
+      <c r="I26" t="b">
+        <v>0</v>
+      </c>
+      <c r="J26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0.1</v>
+      </c>
+      <c r="F27">
+        <v>150</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>30</v>
+      </c>
+      <c r="I27" t="b">
+        <v>1</v>
+      </c>
+      <c r="J27" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:I4 A18:I18 A14:D14 F14:I14 A15:D15 F15:I15 A16:D16 F16:H16 A17:D17 F17:I17 A21:I22 A20:D20 F20:I20 A19:D19 F19:I19 A23:D23 F23:I23 A11:I13 A9:D9 H9:I9 A10:D10 F10:I10 A6:I6 A5:D5 F5:I5 A8:D8 A7:D7 F7:I7 F8:I8" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:J4 A27:J27 A26:H26 J26 A9:J23 A5:H5 J5 A6:H6 J6 A7:H7 J7 A8:H8 J8 A25:J25 A24:H24 J24" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1276,74 +1500,69 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C1" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B2">
         <v>458</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="B3">
         <v>850</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="B4">
         <v>550</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="B5">
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:C1 A5:C5 A2 A3 A4 C4" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:C5" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>